<commit_message>
Upload of full NDA tests
</commit_message>
<xml_diff>
--- a/Simulations/Test 1/Test 1 Data.xlsx
+++ b/Simulations/Test 1/Test 1 Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan Diggins\Desktop\EvolutionaryModeling\Simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan Diggins\Desktop\EvolutionaryModeling\Simulations\Test 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FE65A2-3A77-4748-9AC3-8A8E7911C97A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0349FF05-48DF-404E-AA20-AE92C3AD89F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Test #</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>std.dev</t>
+  </si>
+  <si>
+    <t>Population Growth Over 30 Generations</t>
+  </si>
+  <si>
+    <t>Generation #</t>
   </si>
 </sst>
 </file>
@@ -92,12 +98,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -106,39 +112,234 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -146,15 +347,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -252,7 +474,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$2</c:f>
+              <c:f>Sheet3!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -292,7 +514,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$AG$2</c:f>
+              <c:f>Sheet3!$B$4:$AG$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -404,7 +626,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$3</c:f>
+              <c:f>Sheet3!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -442,7 +664,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$3:$AG$3</c:f>
+              <c:f>Sheet3!$B$5:$AG$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -554,7 +776,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$4</c:f>
+              <c:f>Sheet3!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -592,7 +814,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$4:$AG$4</c:f>
+              <c:f>Sheet3!$B$6:$AG$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -704,7 +926,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$5</c:f>
+              <c:f>Sheet3!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -742,7 +964,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$5:$AG$5</c:f>
+              <c:f>Sheet3!$B$7:$AG$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -854,7 +1076,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$6</c:f>
+              <c:f>Sheet3!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -892,7 +1114,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$6:$AG$6</c:f>
+              <c:f>Sheet3!$B$8:$AG$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1004,7 +1226,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$8</c:f>
+              <c:f>Sheet3!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1014,9 +1236,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1032,7 +1256,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet3!$B$7:$AF$7</c:f>
+                <c:f>Sheet3!$B$10:$AF$10</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="31"/>
@@ -1134,7 +1358,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet3!$B$7:$AF$7</c:f>
+                <c:f>Sheet3!$B$10:$AF$10</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="31"/>
@@ -1247,10 +1471,10 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$8:$AG$8</c:f>
+              <c:f>Sheet3!$B$9:$AF$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1359,7 +1583,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$9</c:f>
+              <c:f>Sheet3!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1383,7 +1607,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$9:$AG$9</c:f>
+              <c:f>Sheet3!$B$11:$AG$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2396,16 +2620,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>36576</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>204870</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>6750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2696,1001 +2920,1164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41EA375-F291-4D75-BF50-D22D46121558}">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
     <col min="3" max="10" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="32" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="13"/>
+    </row>
+    <row r="2" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="16"/>
+    </row>
+    <row r="3" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B3" s="7">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C3" s="17">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D3" s="17">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="E3" s="17">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="F3" s="17">
         <v>4</v>
       </c>
-      <c r="G1">
+      <c r="G3" s="17">
         <v>5</v>
       </c>
-      <c r="H1">
+      <c r="H3" s="17">
         <v>6</v>
       </c>
-      <c r="I1">
+      <c r="I3" s="17">
         <v>7</v>
       </c>
-      <c r="J1">
+      <c r="J3" s="17">
         <v>8</v>
       </c>
-      <c r="K1">
+      <c r="K3" s="17">
         <v>9</v>
       </c>
-      <c r="L1">
+      <c r="L3" s="17">
         <v>10</v>
       </c>
-      <c r="M1">
+      <c r="M3" s="17">
         <v>11</v>
       </c>
-      <c r="N1">
+      <c r="N3" s="17">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="O3" s="17">
         <v>13</v>
       </c>
-      <c r="P1">
+      <c r="P3" s="17">
         <v>14</v>
       </c>
-      <c r="Q1">
+      <c r="Q3" s="17">
         <v>15</v>
       </c>
-      <c r="R1">
+      <c r="R3" s="17">
         <v>16</v>
       </c>
-      <c r="S1">
+      <c r="S3" s="17">
         <v>17</v>
       </c>
-      <c r="T1">
+      <c r="T3" s="17">
         <v>18</v>
       </c>
-      <c r="U1">
+      <c r="U3" s="17">
         <v>19</v>
       </c>
-      <c r="V1">
+      <c r="V3" s="17">
         <v>20</v>
       </c>
-      <c r="W1">
+      <c r="W3" s="17">
         <v>21</v>
       </c>
-      <c r="X1">
+      <c r="X3" s="17">
         <v>22</v>
       </c>
-      <c r="Y1">
+      <c r="Y3" s="17">
         <v>23</v>
       </c>
-      <c r="Z1">
+      <c r="Z3" s="17">
         <v>24</v>
       </c>
-      <c r="AA1">
+      <c r="AA3" s="17">
         <v>25</v>
       </c>
-      <c r="AB1">
+      <c r="AB3" s="17">
         <v>26</v>
       </c>
-      <c r="AC1">
+      <c r="AC3" s="17">
         <v>27</v>
       </c>
-      <c r="AD1">
+      <c r="AD3" s="17">
         <v>28</v>
       </c>
-      <c r="AE1">
+      <c r="AE3" s="17">
         <v>29</v>
       </c>
-      <c r="AF1">
+      <c r="AF3" s="18">
         <v>30</v>
       </c>
-      <c r="AG1">
+      <c r="AG3">
         <v>0.80643722559999997</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="4" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D4" s="8">
         <v>4</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E4" s="8">
         <v>8</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F4" s="8">
         <v>16</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G4" s="8">
         <v>24</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H4" s="8">
         <v>33</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I4" s="8">
         <v>32</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J4" s="8">
         <v>35</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K4" s="8">
         <v>33</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L4" s="8">
         <v>39</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M4" s="8">
         <v>38</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N4" s="8">
         <v>39</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O4" s="8">
         <v>39</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P4" s="8">
         <v>36</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q4" s="8">
         <v>38</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R4" s="8">
         <v>36</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S4" s="8">
         <v>40</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T4" s="8">
         <v>38</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U4" s="8">
         <v>37</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V4" s="8">
         <v>36</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W4" s="8">
         <v>37</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X4" s="8">
         <v>34</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y4" s="8">
         <v>30</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z4" s="8">
         <v>34</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA4" s="8">
         <v>35</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB4" s="8">
         <v>37</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC4" s="8">
         <v>37</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD4" s="8">
         <v>35</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE4" s="8">
         <v>36</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AF4" s="9">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="5" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E5" s="1">
         <v>8</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F5" s="1">
         <v>15</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G5" s="1">
         <v>26</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H5" s="1">
         <v>27</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I5" s="1">
         <v>37</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J5" s="1">
         <v>35</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K5" s="1">
         <v>37</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L5" s="1">
         <v>39</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M5" s="1">
         <v>33</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N5" s="1">
         <v>36</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O5" s="1">
         <v>40</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P5" s="1">
         <v>37</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q5" s="1">
         <v>35</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R5" s="1">
         <v>32</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S5" s="1">
         <v>38</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T5" s="1">
         <v>39</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U5" s="1">
         <v>39</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V5" s="1">
         <v>38</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W5" s="1">
         <v>31</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X5" s="1">
         <v>29</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y5" s="1">
         <v>35</v>
       </c>
-      <c r="Z3" s="4">
+      <c r="Z5" s="1">
         <v>37</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AA5" s="1">
         <v>36</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="AB5" s="1">
         <v>32</v>
       </c>
-      <c r="AC3" s="4">
+      <c r="AC5" s="1">
         <v>36</v>
       </c>
-      <c r="AD3" s="4">
+      <c r="AD5" s="1">
         <v>39</v>
       </c>
-      <c r="AE3" s="4">
+      <c r="AE5" s="1">
         <v>38</v>
       </c>
-      <c r="AF3" s="6">
+      <c r="AF5" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="6" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E6" s="1">
         <v>8</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F6" s="1">
         <v>16</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G6" s="1">
         <v>30</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H6" s="1">
         <v>33</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I6" s="1">
         <v>38</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J6" s="1">
         <v>39</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K6" s="1">
         <v>37</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L6" s="1">
         <v>38</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M6" s="1">
         <v>34</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N6" s="1">
         <v>35</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O6" s="1">
         <v>36</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P6" s="1">
         <v>38</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q6" s="1">
         <v>37</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R6" s="1">
         <v>33</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S6" s="1">
         <v>30</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T6" s="1">
         <v>36</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U6" s="1">
         <v>35</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V6" s="1">
         <v>35</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W6" s="1">
         <v>36</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X6" s="1">
         <v>36</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y6" s="1">
         <v>39</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z6" s="1">
         <v>38</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA6" s="1">
         <v>34</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB6" s="1">
         <v>37</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC6" s="1">
         <v>37</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD6" s="1">
         <v>42</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE6" s="1">
         <v>34</v>
       </c>
-      <c r="AF4" s="5">
+      <c r="AF6" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="7" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D7" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E7" s="1">
         <v>8</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F7" s="1">
         <v>16</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G7" s="1">
         <v>27</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H7" s="1">
         <v>33</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I7" s="1">
         <v>36</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J7" s="1">
         <v>35</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K7" s="1">
         <v>38</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L7" s="1">
         <v>37</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M7" s="1">
         <v>36</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N7" s="1">
         <v>37</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O7" s="1">
         <v>37</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P7" s="1">
         <v>37</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q7" s="1">
         <v>38</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R7" s="1">
         <v>41</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S7" s="1">
         <v>37</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T7" s="1">
         <v>36</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U7" s="1">
         <v>35</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V7" s="1">
         <v>37</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W7" s="1">
         <v>34</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X7" s="1">
         <v>33</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y7" s="1">
         <v>31</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z7" s="1">
         <v>36</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AA7" s="1">
         <v>32</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AB7" s="1">
         <v>37</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AC7" s="1">
         <v>36</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AD7" s="1">
         <v>35</v>
       </c>
-      <c r="AE5" s="4">
+      <c r="AE7" s="1">
         <v>36</v>
       </c>
-      <c r="AF5" s="6">
+      <c r="AF7" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="8" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D8" s="1">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E8" s="1">
         <v>8</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F8" s="1">
         <v>16</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G8" s="1">
         <v>27</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H8" s="1">
         <v>38</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I8" s="1">
         <v>39</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J8" s="1">
         <v>34</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K8" s="1">
         <v>37</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L8" s="1">
         <v>36</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M8" s="1">
         <v>33</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N8" s="1">
         <v>32</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O8" s="1">
         <v>35</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P8" s="1">
         <v>35</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q8" s="1">
         <v>40</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R8" s="1">
         <v>40</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S8" s="1">
         <v>37</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T8" s="1">
         <v>34</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U8" s="1">
         <v>34</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V8" s="1">
         <v>34</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W8" s="1">
         <v>41</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X8" s="1">
         <v>38</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y8" s="1">
         <v>36</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z8" s="1">
         <v>40</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA8" s="1">
         <v>40</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB8" s="1">
         <v>37</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AC8" s="1">
         <v>37</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD8" s="1">
         <v>38</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AE8" s="1">
         <v>39</v>
       </c>
-      <c r="AF6" s="5">
+      <c r="AF8" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="9" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5">
+        <f>AVERAGE(B4:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C4:C8)</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <f>AVERAGE(D4:D8)</f>
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <f>AVERAGE(E4:E8)</f>
+        <v>8</v>
+      </c>
+      <c r="F9" s="5">
+        <f>AVERAGE(F4:F8)</f>
+        <v>15.8</v>
+      </c>
+      <c r="G9" s="5">
+        <f>AVERAGE(G4:G8)</f>
+        <v>26.8</v>
+      </c>
+      <c r="H9" s="5">
+        <f>AVERAGE(H4:H8)</f>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="I9" s="5">
+        <f>AVERAGE(I4:I8)</f>
+        <v>36.4</v>
+      </c>
+      <c r="J9" s="5">
+        <f>AVERAGE(J4:J8)</f>
+        <v>35.6</v>
+      </c>
+      <c r="K9" s="5">
+        <f>AVERAGE(K4:K8)</f>
+        <v>36.4</v>
+      </c>
+      <c r="L9" s="5">
+        <f>AVERAGE(L4:L8)</f>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="M9" s="5">
+        <f>AVERAGE(M4:M8)</f>
+        <v>34.799999999999997</v>
+      </c>
+      <c r="N9" s="5">
+        <f>AVERAGE(N4:N8)</f>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="O9" s="5">
+        <f>AVERAGE(O4:O8)</f>
+        <v>37.4</v>
+      </c>
+      <c r="P9" s="5">
+        <f>AVERAGE(P4:P8)</f>
+        <v>36.6</v>
+      </c>
+      <c r="Q9" s="5">
+        <f>AVERAGE(Q4:Q8)</f>
+        <v>37.6</v>
+      </c>
+      <c r="R9" s="5">
+        <f>AVERAGE(R4:R8)</f>
+        <v>36.4</v>
+      </c>
+      <c r="S9" s="5">
+        <f>AVERAGE(S4:S8)</f>
+        <v>36.4</v>
+      </c>
+      <c r="T9" s="5">
+        <f>AVERAGE(T4:T8)</f>
+        <v>36.6</v>
+      </c>
+      <c r="U9" s="5">
+        <f>AVERAGE(U4:U8)</f>
+        <v>36</v>
+      </c>
+      <c r="V9" s="5">
+        <f>AVERAGE(V4:V8)</f>
+        <v>36</v>
+      </c>
+      <c r="W9" s="5">
+        <f>AVERAGE(W4:W8)</f>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="X9" s="5">
+        <f>AVERAGE(X4:X8)</f>
+        <v>34</v>
+      </c>
+      <c r="Y9" s="5">
+        <f>AVERAGE(Y4:Y8)</f>
+        <v>34.200000000000003</v>
+      </c>
+      <c r="Z9" s="5">
+        <f>AVERAGE(Z4:Z8)</f>
+        <v>37</v>
+      </c>
+      <c r="AA9" s="5">
+        <f>AVERAGE(AA4:AA8)</f>
+        <v>35.4</v>
+      </c>
+      <c r="AB9" s="5">
+        <f>AVERAGE(AB4:AB8)</f>
+        <v>36</v>
+      </c>
+      <c r="AC9" s="5">
+        <f>AVERAGE(AC4:AC8)</f>
+        <v>36.6</v>
+      </c>
+      <c r="AD9" s="5">
+        <f>AVERAGE(AD4:AD8)</f>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="AE9" s="5">
+        <f>AVERAGE(AE4:AE8)</f>
+        <v>36.6</v>
+      </c>
+      <c r="AF9" s="6">
+        <f>AVERAGE(AF4:AF8)</f>
+        <v>38.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7">
-        <f>_xlfn.STDEV.P(B2:B6)</f>
+      <c r="B10" s="1">
+        <f>_xlfn.STDEV.P(B4:B8)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="7">
-        <f t="shared" ref="C7:AF7" si="0">_xlfn.STDEV.P(C2:C6)</f>
+      <c r="C10" s="1">
+        <f t="shared" ref="C10:AF10" si="0">_xlfn.STDEV.P(C4:C8)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>0.39999999999999997</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>1.9390719429665315</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>3.4871191548325386</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>2.4166091947189146</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
         <v>1.7435595774162693</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
         <v>1.7435595774162693</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L10" s="1">
         <f t="shared" si="0"/>
         <v>1.16619037896906</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M10" s="1">
         <f t="shared" si="0"/>
         <v>1.9390719429665315</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>2.3151673805580448</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O10" s="1">
         <f t="shared" si="0"/>
         <v>1.8547236990991407</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P10" s="1">
         <f t="shared" si="0"/>
         <v>1.0198039027185568</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q10" s="1">
         <f t="shared" si="0"/>
         <v>1.6248076809271923</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R10" s="1">
         <f t="shared" si="0"/>
         <v>3.6110940170535577</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S10" s="1">
         <f t="shared" si="0"/>
         <v>3.3823069050575523</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T10" s="1">
         <f t="shared" si="0"/>
         <v>1.7435595774162693</v>
       </c>
-      <c r="U7" s="7">
+      <c r="U10" s="1">
         <f t="shared" si="0"/>
         <v>1.7888543819998317</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V10" s="1">
         <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W10" s="1">
         <f t="shared" si="0"/>
         <v>3.3105890714493702</v>
       </c>
-      <c r="X7" s="7">
+      <c r="X10" s="1">
         <f t="shared" si="0"/>
         <v>3.03315017762062</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Y10" s="1">
         <f t="shared" si="0"/>
         <v>3.3105890714493698</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z10" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AA7" s="7">
+      <c r="AA10" s="1">
         <f t="shared" si="0"/>
         <v>2.6532998322843202</v>
       </c>
-      <c r="AB7" s="7">
+      <c r="AB10" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="AC10" s="1">
         <f t="shared" si="0"/>
         <v>0.4898979485566356</v>
       </c>
-      <c r="AD7" s="7">
+      <c r="AD10" s="1">
         <f t="shared" si="0"/>
         <v>2.6381811916545836</v>
       </c>
-      <c r="AE7" s="7">
+      <c r="AE10" s="1">
         <f t="shared" si="0"/>
         <v>1.7435595774162693</v>
       </c>
-      <c r="AF7" s="7">
+      <c r="AF10" s="2">
         <f t="shared" si="0"/>
         <v>2.2449944320643649</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <f>AVERAGE(B2:B6)</f>
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:AF8" si="1">AVERAGE(C2:C6)</f>
+    <row r="11" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="B11" s="1">
+        <f>(36)/(1+EXP(-1*$AG$3*(B$3-4.40871)))</f>
+        <v>1.0000001950418329</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:AF11" si="1">(36)/(1+EXP(-1*$AG$3*(C$3-4.40871)))</f>
+        <v>2.1653353041950743</v>
+      </c>
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E8">
+        <v>4.5135496104035493</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F8">
+        <v>8.749759158285082</v>
+      </c>
+      <c r="F11" s="1">
         <f t="shared" si="1"/>
-        <v>15.8</v>
-      </c>
-      <c r="G8">
+        <v>15.06017541374244</v>
+      </c>
+      <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>26.8</v>
-      </c>
-      <c r="H8">
+        <v>22.212036005840922</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>32.799999999999997</v>
-      </c>
-      <c r="I8">
+        <v>28.188245588249028</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="J8">
+        <v>32.036374128531108</v>
+      </c>
+      <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>35.6</v>
-      </c>
-      <c r="K8">
+        <v>34.115608311070702</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="L8">
+        <v>35.133617459297199</v>
+      </c>
+      <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>37.799999999999997</v>
-      </c>
-      <c r="M8">
+        <v>35.607984732473454</v>
+      </c>
+      <c r="M11" s="1">
         <f t="shared" si="1"/>
-        <v>34.799999999999997</v>
-      </c>
-      <c r="N8">
+        <v>35.823925072904473</v>
+      </c>
+      <c r="N11" s="1">
         <f t="shared" si="1"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="O8">
+        <v>35.921178682285628</v>
+      </c>
+      <c r="O11" s="1">
         <f t="shared" si="1"/>
-        <v>37.4</v>
-      </c>
-      <c r="P8">
+        <v>35.964767850793898</v>
+      </c>
+      <c r="P11" s="1">
         <f t="shared" si="1"/>
-        <v>36.6</v>
-      </c>
-      <c r="Q8">
+        <v>35.984262228295457</v>
+      </c>
+      <c r="Q11" s="1">
         <f t="shared" si="1"/>
-        <v>37.6</v>
-      </c>
-      <c r="R8">
+        <v>35.992972236914881</v>
+      </c>
+      <c r="R11" s="1">
         <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="S8">
+        <v>35.996862145449278</v>
+      </c>
+      <c r="S11" s="1">
         <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="T8">
+        <v>35.998599050351409</v>
+      </c>
+      <c r="T11" s="1">
         <f t="shared" si="1"/>
-        <v>36.6</v>
-      </c>
-      <c r="U8">
+        <v>35.999374538409207</v>
+      </c>
+      <c r="U11" s="1">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="V8">
+        <v>35.999720762600504</v>
+      </c>
+      <c r="V11" s="1">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="W8">
+        <v>35.999875335094416</v>
+      </c>
+      <c r="W11" s="1">
         <f t="shared" si="1"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="X8">
+        <v>35.999944343767076</v>
+      </c>
+      <c r="X11" s="1">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="Y8">
+        <v>35.999975152486087</v>
+      </c>
+      <c r="Y11" s="1">
         <f t="shared" si="1"/>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="Z8">
+        <v>35.999988906926994</v>
+      </c>
+      <c r="Z11" s="1">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="AA8">
+        <v>35.999995047543059</v>
+      </c>
+      <c r="AA11" s="1">
         <f t="shared" si="1"/>
-        <v>35.4</v>
-      </c>
-      <c r="AB8">
+        <v>35.999997788996126</v>
+      </c>
+      <c r="AB11" s="1">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="AC8">
+        <v>35.999999012906521</v>
+      </c>
+      <c r="AC11" s="1">
         <f t="shared" si="1"/>
-        <v>36.6</v>
-      </c>
-      <c r="AD8">
+        <v>35.999999559316237</v>
+      </c>
+      <c r="AD11" s="1">
         <f t="shared" si="1"/>
-        <v>37.799999999999997</v>
-      </c>
-      <c r="AE8">
+        <v>35.999999803258568</v>
+      </c>
+      <c r="AE11" s="1">
         <f t="shared" si="1"/>
-        <v>36.6</v>
-      </c>
-      <c r="AF8">
+        <v>35.999999912165613</v>
+      </c>
+      <c r="AF11" s="2">
         <f t="shared" si="1"/>
-        <v>38.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <f>(36)/(1+EXP(-1*$AG$1*(B$1-4.40871)))</f>
-        <v>1.0000001950418329</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:AF9" si="2">(36)/(1+EXP(-1*$AG$1*(C$1-4.40871)))</f>
-        <v>2.1653353041950743</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>4.5135496104035493</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>8.749759158285082</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>15.06017541374244</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>22.212036005840922</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>28.188245588249028</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>32.036374128531108</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>34.115608311070702</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
-        <v>35.133617459297199</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>35.607984732473454</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>35.823925072904473</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="2"/>
-        <v>35.921178682285628</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="2"/>
-        <v>35.964767850793898</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="2"/>
-        <v>35.984262228295457</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
-        <v>35.992972236914881</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="2"/>
-        <v>35.996862145449278</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="2"/>
-        <v>35.998599050351409</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="2"/>
-        <v>35.999374538409207</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="2"/>
-        <v>35.999720762600504</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="2"/>
-        <v>35.999875335094416</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="2"/>
-        <v>35.999944343767076</v>
-      </c>
-      <c r="X9">
-        <f t="shared" si="2"/>
-        <v>35.999975152486087</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" si="2"/>
-        <v>35.999988906926994</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="2"/>
-        <v>35.999995047543059</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="2"/>
-        <v>35.999997788996126</v>
-      </c>
-      <c r="AB9">
-        <f t="shared" si="2"/>
-        <v>35.999999012906521</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="2"/>
-        <v>35.999999559316237</v>
-      </c>
-      <c r="AD9">
-        <f t="shared" si="2"/>
-        <v>35.999999803258568</v>
-      </c>
-      <c r="AE9">
-        <f t="shared" si="2"/>
-        <v>35.999999912165613</v>
-      </c>
-      <c r="AF9">
-        <f t="shared" si="2"/>
         <v>35.999999960786703</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="B2:AF2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B4:AF4">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:AF5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:AF6">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:AF7">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:AF8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:AF9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:AF11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B9:AF10" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>